<commit_message>
Remplacement de la notion d'artiste pour la notion de type sur les nodes
</commit_message>
<xml_diff>
--- a/tools/talend/Communaute_BI.xlsx
+++ b/tools/talend/Communaute_BI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="Liste" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Client">Liste!$G$2:$G$8</definedName>
-    <definedName name="Colab">Colab!$A$2:$A$5</definedName>
+    <definedName name="Client">Liste!$G$2:$G$9</definedName>
+    <definedName name="Colab">Colab!$A$2:$A$6</definedName>
     <definedName name="Concept">Liste!$D$2:$D$6</definedName>
     <definedName name="Niveau">Liste!$J$2:$J$6</definedName>
     <definedName name="Outil">Liste!$A$2:$A$6</definedName>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Outil</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>KIABI</t>
+  </si>
+  <si>
+    <t>Mehdi Tajmouati</t>
+  </si>
+  <si>
+    <t>MTI</t>
+  </si>
+  <si>
+    <t>CASA</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,32 +665,55 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9">
       <formula1>Outil</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
       <formula1>Concept</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9">
       <formula1>Client</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8 C2:C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9 C2:C9">
       <formula1>Niveau</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A9">
       <formula1>Colab</formula1>
     </dataValidation>
   </dataValidations>
@@ -692,21 +724,21 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Liste!N3</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>Liste!N4</xm:f>
+          </x14:formula2>
+          <xm:sqref>G9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Liste!N2</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>Liste!N3</xm:f>
           </x14:formula2>
-          <xm:sqref>G6:G7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Liste!N3</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>Liste!N4</xm:f>
-          </x14:formula2>
-          <xm:sqref>G8</xm:sqref>
+          <xm:sqref>G6:G8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -743,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,9 +818,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -797,10 +837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +929,7 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -900,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -908,11 +948,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>